<commit_message>
added basic functionality to populate database with data from a spreadsheet, then show that data in a GridView
</commit_message>
<xml_diff>
--- a/ExcelToSQLServer/SpreadSheets/dataSource.xlsx
+++ b/ExcelToSQLServer/SpreadSheets/dataSource.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>Oaks</t>
+  </si>
+  <si>
+    <t>Calvin</t>
+  </si>
+  <si>
+    <t>NoKlein</t>
+  </si>
+  <si>
+    <t>Anoder</t>
+  </si>
+  <si>
+    <t>Naame</t>
   </si>
 </sst>
 </file>
@@ -402,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,7 +487,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="0"/>
+        <f>ROW(A5)</f>
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -483,6 +495,30 @@
       </c>
       <c r="C6" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f>ROW(A6)</f>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f>ROW(A7)</f>
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bug with stored procedure not being called. The program should now update the database whenever a new record is added to the spreadsheet
</commit_message>
<xml_diff>
--- a/ExcelToSQLServer/SpreadSheets/dataSource.xlsx
+++ b/ExcelToSQLServer/SpreadSheets/dataSource.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>Naame</t>
+  </si>
+  <si>
+    <t>Ryan</t>
+  </si>
+  <si>
+    <t>Rain</t>
   </si>
 </sst>
 </file>
@@ -414,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,6 +527,17 @@
         <v>16</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
removed the Entity Data Model as it wasn't needed for this project. Also method call to mergeCommand to execute its query as it was accidently removed.
</commit_message>
<xml_diff>
--- a/ExcelToSQLServer/SpreadSheets/dataSource.xlsx
+++ b/ExcelToSQLServer/SpreadSheets/dataSource.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>ID</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>Rain</t>
+  </si>
+  <si>
+    <t>Rachel</t>
+  </si>
+  <si>
+    <t>Milo</t>
   </si>
 </sst>
 </file>
@@ -420,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,6 +544,17 @@
         <v>18</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>